<commit_message>
Finishing homogenizing geo and some other details
</commit_message>
<xml_diff>
--- a/code/lista_homogen_codes_geo.xlsx
+++ b/code/lista_homogen_codes_geo.xlsx
@@ -518,9 +518,6 @@
     <t>19020</t>
   </si>
   <si>
-    <t>codigo_2012_2016</t>
-  </si>
-  <si>
     <t>0101</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>1901</t>
+  </si>
+  <si>
+    <t>codigo_2012_2014</t>
   </si>
 </sst>
 </file>
@@ -784,9 +784,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -796,6 +793,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,28 +1088,28 @@
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>164</v>
+      <c r="F1" s="13" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1123,9 +1123,9 @@
         <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -1133,7 +1133,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B3">
@@ -1143,7 +1143,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1151,7 +1151,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
+      <c r="A4" s="14"/>
       <c r="B4">
         <v>2</v>
       </c>
@@ -1159,9 +1159,9 @@
         <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E4" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1169,7 +1169,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="14"/>
       <c r="B5">
         <v>2</v>
       </c>
@@ -1177,9 +1177,9 @@
         <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E5" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1187,7 +1187,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="14"/>
       <c r="B6">
         <v>2</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>29</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>900</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1203,7 +1203,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="14" t="s">
         <v>106</v>
       </c>
       <c r="B7">
@@ -1213,7 +1213,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1221,7 +1221,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="14"/>
       <c r="B8">
         <v>3</v>
       </c>
@@ -1229,9 +1229,9 @@
         <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E8" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1239,7 +1239,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+      <c r="A9" s="14"/>
       <c r="B9">
         <v>3</v>
       </c>
@@ -1247,9 +1247,9 @@
         <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1257,7 +1257,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="14"/>
       <c r="B10">
         <v>3</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>32</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="4" t="s">
@@ -1273,7 +1273,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="14"/>
       <c r="B11">
         <v>3</v>
       </c>
@@ -1281,9 +1281,9 @@
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="E11" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="4" t="s">
@@ -1291,7 +1291,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="14"/>
       <c r="B12">
         <v>3</v>
       </c>
@@ -1299,9 +1299,9 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1309,7 +1309,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="14"/>
       <c r="B13">
         <v>3</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>35</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1325,7 +1325,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="14"/>
       <c r="B14">
         <v>3</v>
       </c>
@@ -1333,9 +1333,9 @@
         <v>36</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="E14" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1343,7 +1343,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="14"/>
       <c r="B15">
         <v>3</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>37</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="14"/>
       <c r="B16">
         <v>3</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>38</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>900</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -1375,7 +1375,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B17">
@@ -1385,7 +1385,7 @@
         <v>26</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1393,7 +1393,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="14"/>
       <c r="B18">
         <v>4</v>
       </c>
@@ -1401,9 +1401,9 @@
         <v>39</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E18" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
@@ -1411,7 +1411,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="14"/>
       <c r="B19">
         <v>4</v>
       </c>
@@ -1419,9 +1419,9 @@
         <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E19" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F19" s="4" t="s">
@@ -1429,7 +1429,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="14"/>
       <c r="B20">
         <v>4</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>41</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="12">
+      <c r="E20" s="11">
         <v>900</v>
       </c>
       <c r="F20" s="5" t="s">
@@ -1445,7 +1445,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="14" t="s">
         <v>108</v>
       </c>
       <c r="B21">
@@ -1455,7 +1455,7 @@
         <v>26</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -1463,7 +1463,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="14"/>
       <c r="B22">
         <v>5</v>
       </c>
@@ -1471,9 +1471,9 @@
         <v>42</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E22" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F22" s="4" t="s">
@@ -1481,7 +1481,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="14"/>
       <c r="B23">
         <v>5</v>
       </c>
@@ -1489,9 +1489,9 @@
         <v>43</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E23" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="14"/>
       <c r="B24">
         <v>5</v>
       </c>
@@ -1507,9 +1507,9 @@
         <v>44</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E24" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="4" t="s">
@@ -1517,7 +1517,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="14"/>
       <c r="B25">
         <v>5</v>
       </c>
@@ -1525,7 +1525,7 @@
         <v>45</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -1533,7 +1533,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="14"/>
       <c r="B26">
         <v>5</v>
       </c>
@@ -1541,9 +1541,9 @@
         <v>46</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E26" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="E26" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F26" s="4" t="s">
@@ -1551,7 +1551,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="14"/>
       <c r="B27">
         <v>5</v>
       </c>
@@ -1559,9 +1559,9 @@
         <v>47</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="E27" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E27" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1569,7 +1569,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="14"/>
       <c r="B28">
         <v>5</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>48</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -1585,7 +1585,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="14"/>
       <c r="B29">
         <v>5</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>49</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F29" s="4" t="s">
@@ -1601,7 +1601,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="14"/>
       <c r="B30">
         <v>5</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>50</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="12">
+      <c r="E30" s="11">
         <v>900</v>
       </c>
       <c r="F30" s="5" t="s">
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B31">
@@ -1627,7 +1627,7 @@
         <v>26</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F31" s="3" t="s">
@@ -1635,7 +1635,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="14"/>
       <c r="B32">
         <v>6</v>
       </c>
@@ -1643,9 +1643,9 @@
         <v>51</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E32" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -1653,7 +1653,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="14"/>
       <c r="B33">
         <v>6</v>
       </c>
@@ -1661,9 +1661,9 @@
         <v>52</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E33" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F33" s="4" t="s">
@@ -1671,7 +1671,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="14"/>
       <c r="B34">
         <v>6</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>53</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="12">
+      <c r="E34" s="11">
         <v>900</v>
       </c>
       <c r="F34" s="5" t="s">
@@ -1687,7 +1687,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="14" t="s">
         <v>110</v>
       </c>
       <c r="B35">
@@ -1697,7 +1697,7 @@
         <v>26</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -1705,7 +1705,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="14"/>
       <c r="B36">
         <v>7</v>
       </c>
@@ -1713,9 +1713,9 @@
         <v>54</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E36" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E36" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F36" s="4" t="s">
@@ -1723,7 +1723,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="14"/>
       <c r="B37">
         <v>7</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>55</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="12">
+      <c r="E37" s="11">
         <v>900</v>
       </c>
       <c r="F37" s="5" t="s">
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B38">
@@ -1749,7 +1749,7 @@
         <v>26</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="10" t="s">
+      <c r="E38" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -1757,7 +1757,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="14"/>
       <c r="B39">
         <v>8</v>
       </c>
@@ -1765,9 +1765,9 @@
         <v>56</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -1775,7 +1775,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="14"/>
       <c r="B40">
         <v>8</v>
       </c>
@@ -1783,9 +1783,9 @@
         <v>57</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E40" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -1793,7 +1793,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="14"/>
       <c r="B41">
         <v>8</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>58</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="12">
+      <c r="E41" s="11">
         <v>900</v>
       </c>
       <c r="F41" s="5" t="s">
@@ -1809,7 +1809,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B42">
@@ -1819,7 +1819,7 @@
         <v>26</v>
       </c>
       <c r="D42" s="1"/>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="3" t="s">
@@ -1827,7 +1827,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="14"/>
       <c r="B43">
         <v>9</v>
       </c>
@@ -1835,9 +1835,9 @@
         <v>59</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="E43" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F43" s="4" t="s">
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="14"/>
       <c r="B44">
         <v>9</v>
       </c>
@@ -1853,9 +1853,9 @@
         <v>60</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E44" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F44" s="4" t="s">
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="14"/>
       <c r="B45">
         <v>9</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>61</v>
       </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="12">
+      <c r="E45" s="11">
         <v>900</v>
       </c>
       <c r="F45" s="5" t="s">
@@ -1879,7 +1879,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="14" t="s">
         <v>112</v>
       </c>
       <c r="B46">
@@ -1889,7 +1889,7 @@
         <v>26</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1897,7 +1897,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="14"/>
       <c r="B47">
         <v>10</v>
       </c>
@@ -1905,9 +1905,9 @@
         <v>62</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E47" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="E47" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -1915,7 +1915,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
+      <c r="A48" s="14"/>
       <c r="B48">
         <v>10</v>
       </c>
@@ -1923,9 +1923,9 @@
         <v>63</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E48" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="E48" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -1933,7 +1933,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
+      <c r="A49" s="14"/>
       <c r="B49">
         <v>10</v>
       </c>
@@ -1941,9 +1941,9 @@
         <v>64</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E49" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F49" s="4" t="s">
@@ -1951,7 +1951,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
+      <c r="A50" s="14"/>
       <c r="B50">
         <v>10</v>
       </c>
@@ -1959,9 +1959,9 @@
         <v>65</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E50" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F50" s="4" t="s">
@@ -1969,7 +1969,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
+      <c r="A51" s="14"/>
       <c r="B51">
         <v>10</v>
       </c>
@@ -1977,9 +1977,9 @@
         <v>66</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E51" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="E51" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F51" s="4" t="s">
@@ -1987,7 +1987,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
+      <c r="A52" s="14"/>
       <c r="B52">
         <v>10</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>67</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F52" s="4" t="s">
@@ -2003,7 +2003,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
+      <c r="A53" s="14"/>
       <c r="B53">
         <v>10</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>68</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="12">
+      <c r="E53" s="11">
         <v>900</v>
       </c>
       <c r="F53" s="5" t="s">
@@ -2019,7 +2019,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="A54" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B54">
@@ -2029,7 +2029,7 @@
         <v>26</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -2037,7 +2037,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
+      <c r="A55" s="14"/>
       <c r="B55">
         <v>11</v>
       </c>
@@ -2045,9 +2045,9 @@
         <v>69</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E55" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="E55" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F55" s="4" t="s">
@@ -2055,7 +2055,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
+      <c r="A56" s="14"/>
       <c r="B56">
         <v>11</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>70</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="11" t="s">
+      <c r="E56" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F56" s="4" t="s">
@@ -2071,7 +2071,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7"/>
+      <c r="A57" s="14"/>
       <c r="B57">
         <v>11</v>
       </c>
@@ -2079,9 +2079,9 @@
         <v>71</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E57" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E57" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F57" s="4" t="s">
@@ -2089,7 +2089,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="7"/>
+      <c r="A58" s="14"/>
       <c r="B58">
         <v>11</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>72</v>
       </c>
       <c r="D58" s="1"/>
-      <c r="E58" s="12">
+      <c r="E58" s="11">
         <v>900</v>
       </c>
       <c r="F58" s="5" t="s">
@@ -2105,7 +2105,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="14" t="s">
         <v>114</v>
       </c>
       <c r="B59">
@@ -2115,7 +2115,7 @@
         <v>26</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F59" s="3" t="s">
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
+      <c r="A60" s="14"/>
       <c r="B60">
         <v>12</v>
       </c>
@@ -2131,9 +2131,9 @@
         <v>73</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E60" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="E60" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F60" s="4" t="s">
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="7"/>
+      <c r="A61" s="14"/>
       <c r="B61">
         <v>12</v>
       </c>
@@ -2149,9 +2149,9 @@
         <v>74</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E61" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="E61" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F61" s="4" t="s">
@@ -2159,7 +2159,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="7"/>
+      <c r="A62" s="14"/>
       <c r="B62">
         <v>12</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>75</v>
       </c>
       <c r="D62" s="1"/>
-      <c r="E62" s="12">
+      <c r="E62" s="11">
         <v>900</v>
       </c>
       <c r="F62" s="5" t="s">
@@ -2175,7 +2175,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B63">
@@ -2185,7 +2185,7 @@
         <v>26</v>
       </c>
       <c r="D63" s="1"/>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -2193,7 +2193,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="7"/>
+      <c r="A64" s="14"/>
       <c r="B64">
         <v>13</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="D64" s="1">
         <v>1301</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E64" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -2211,7 +2211,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="7"/>
+      <c r="A65" s="14"/>
       <c r="B65">
         <v>13</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="D65" s="1">
         <v>1302</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E65" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F65" s="4" t="s">
@@ -2229,7 +2229,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="7"/>
+      <c r="A66" s="14"/>
       <c r="B66">
         <v>13</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>77</v>
       </c>
       <c r="D66" s="1"/>
-      <c r="E66" s="12">
+      <c r="E66" s="11">
         <v>900</v>
       </c>
       <c r="F66" s="5" t="s">
@@ -2245,7 +2245,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B67">
@@ -2255,7 +2255,7 @@
         <v>26</v>
       </c>
       <c r="D67" s="1"/>
-      <c r="E67" s="10" t="s">
+      <c r="E67" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -2263,7 +2263,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="7"/>
+      <c r="A68" s="14"/>
       <c r="B68">
         <v>14</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>78</v>
       </c>
       <c r="D68" s="1"/>
-      <c r="E68" s="11" t="s">
+      <c r="E68" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F68" s="4" t="s">
@@ -2279,7 +2279,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="7"/>
+      <c r="A69" s="14"/>
       <c r="B69">
         <v>14</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>79</v>
       </c>
       <c r="D69" s="1"/>
-      <c r="E69" s="11" t="s">
+      <c r="E69" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F69" s="4" t="s">
@@ -2295,7 +2295,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="7"/>
+      <c r="A70" s="14"/>
       <c r="B70">
         <v>14</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>80</v>
       </c>
       <c r="D70" s="1"/>
-      <c r="E70" s="11" t="s">
+      <c r="E70" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F70" s="4" t="s">
@@ -2311,7 +2311,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="7"/>
+      <c r="A71" s="14"/>
       <c r="B71">
         <v>14</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>81</v>
       </c>
       <c r="D71" s="1"/>
-      <c r="E71" s="11" t="s">
+      <c r="E71" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F71" s="4" t="s">
@@ -2327,7 +2327,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="7"/>
+      <c r="A72" s="14"/>
       <c r="B72">
         <v>14</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>82</v>
       </c>
       <c r="D72" s="1"/>
-      <c r="E72" s="11" t="s">
+      <c r="E72" s="10" t="s">
         <v>14</v>
       </c>
       <c r="F72" s="4" t="s">
@@ -2343,7 +2343,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="7"/>
+      <c r="A73" s="14"/>
       <c r="B73">
         <v>14</v>
       </c>
@@ -2351,9 +2351,9 @@
         <v>83</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E73" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F73" s="4" t="s">
@@ -2361,7 +2361,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="7"/>
+      <c r="A74" s="14"/>
       <c r="B74">
         <v>14</v>
       </c>
@@ -2369,9 +2369,9 @@
         <v>84</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="E74" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="E74" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F74" s="4" t="s">
@@ -2379,7 +2379,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="7"/>
+      <c r="A75" s="14"/>
       <c r="B75">
         <v>14</v>
       </c>
@@ -2387,9 +2387,9 @@
         <v>85</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E75" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E75" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F75" s="4" t="s">
@@ -2397,7 +2397,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="7"/>
+      <c r="A76" s="14"/>
       <c r="B76">
         <v>14</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>86</v>
       </c>
       <c r="D76" s="1"/>
-      <c r="E76" s="12">
+      <c r="E76" s="11">
         <v>900</v>
       </c>
       <c r="F76" s="5" t="s">
@@ -2413,7 +2413,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="14" t="s">
         <v>115</v>
       </c>
       <c r="B77">
@@ -2423,7 +2423,7 @@
         <v>26</v>
       </c>
       <c r="D77" s="1"/>
-      <c r="E77" s="10" t="s">
+      <c r="E77" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F77" s="3" t="s">
@@ -2431,7 +2431,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="7"/>
+      <c r="A78" s="14"/>
       <c r="B78">
         <v>15</v>
       </c>
@@ -2439,9 +2439,9 @@
         <v>87</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E78" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E78" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F78" s="4" t="s">
@@ -2449,7 +2449,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="7"/>
+      <c r="A79" s="14"/>
       <c r="B79">
         <v>15</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>88</v>
       </c>
       <c r="D79" s="1"/>
-      <c r="E79" s="11" t="s">
+      <c r="E79" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F79" s="4" t="s">
@@ -2465,7 +2465,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="7"/>
+      <c r="A80" s="14"/>
       <c r="B80">
         <v>15</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>89</v>
       </c>
       <c r="D80" s="1"/>
-      <c r="E80" s="12">
+      <c r="E80" s="11">
         <v>900</v>
       </c>
       <c r="F80" s="5" t="s">
@@ -2481,7 +2481,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="14" t="s">
         <v>116</v>
       </c>
       <c r="B81">
@@ -2491,7 +2491,7 @@
         <v>26</v>
       </c>
       <c r="D81" s="1"/>
-      <c r="E81" s="10" t="s">
+      <c r="E81" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F81" s="3" t="s">
@@ -2499,7 +2499,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="7"/>
+      <c r="A82" s="14"/>
       <c r="B82">
         <v>16</v>
       </c>
@@ -2507,9 +2507,9 @@
         <v>90</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E82" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E82" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F82" s="4" t="s">
@@ -2517,7 +2517,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="7"/>
+      <c r="A83" s="14"/>
       <c r="B83">
         <v>16</v>
       </c>
@@ -2525,9 +2525,9 @@
         <v>91</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E83" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="E83" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F83" s="4" t="s">
@@ -2535,7 +2535,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="7"/>
+      <c r="A84" s="14"/>
       <c r="B84">
         <v>16</v>
       </c>
@@ -2543,9 +2543,9 @@
         <v>92</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E84" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="E84" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F84" s="4" t="s">
@@ -2553,7 +2553,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="7"/>
+      <c r="A85" s="14"/>
       <c r="B85">
         <v>16</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>93</v>
       </c>
       <c r="D85" s="1"/>
-      <c r="E85" s="11" t="s">
+      <c r="E85" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F85" s="4" t="s">
@@ -2569,7 +2569,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="7"/>
+      <c r="A86" s="14"/>
       <c r="B86">
         <v>16</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>94</v>
       </c>
       <c r="D86" s="1"/>
-      <c r="E86" s="11" t="s">
+      <c r="E86" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F86" s="4" t="s">
@@ -2585,7 +2585,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="7"/>
+      <c r="A87" s="14"/>
       <c r="B87">
         <v>16</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>95</v>
       </c>
       <c r="D87" s="1"/>
-      <c r="E87" s="12">
+      <c r="E87" s="11">
         <v>900</v>
       </c>
       <c r="F87" s="5" t="s">
@@ -2601,7 +2601,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="14" t="s">
         <v>117</v>
       </c>
       <c r="B88">
@@ -2611,7 +2611,7 @@
         <v>26</v>
       </c>
       <c r="D88" s="1"/>
-      <c r="E88" s="10" t="s">
+      <c r="E88" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F88" s="3" t="s">
@@ -2619,7 +2619,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="7"/>
+      <c r="A89" s="14"/>
       <c r="B89">
         <v>17</v>
       </c>
@@ -2627,9 +2627,9 @@
         <v>96</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E89" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F89" s="4" t="s">
@@ -2637,7 +2637,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="7"/>
+      <c r="A90" s="14"/>
       <c r="B90">
         <v>17</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>97</v>
       </c>
       <c r="D90" s="1"/>
-      <c r="E90" s="11" t="s">
+      <c r="E90" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F90" s="4" t="s">
@@ -2653,7 +2653,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="7"/>
+      <c r="A91" s="14"/>
       <c r="B91">
         <v>17</v>
       </c>
@@ -2661,7 +2661,7 @@
         <v>45</v>
       </c>
       <c r="D91" s="1"/>
-      <c r="E91" s="11" t="s">
+      <c r="E91" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F91" s="4" t="s">
@@ -2669,7 +2669,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="7"/>
+      <c r="A92" s="14"/>
       <c r="B92">
         <v>17</v>
       </c>
@@ -2677,9 +2677,9 @@
         <v>98</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E92" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="E92" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F92" s="4" t="s">
@@ -2687,7 +2687,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="7"/>
+      <c r="A93" s="14"/>
       <c r="B93">
         <v>17</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>99</v>
       </c>
       <c r="D93" s="1"/>
-      <c r="E93" s="12">
+      <c r="E93" s="11">
         <v>900</v>
       </c>
       <c r="F93" s="5" t="s">
@@ -2703,7 +2703,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="14" t="s">
         <v>118</v>
       </c>
       <c r="B94">
@@ -2713,7 +2713,7 @@
         <v>26</v>
       </c>
       <c r="D94" s="1"/>
-      <c r="E94" s="10" t="s">
+      <c r="E94" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F94" s="3" t="s">
@@ -2721,7 +2721,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="7"/>
+      <c r="A95" s="14"/>
       <c r="B95">
         <v>18</v>
       </c>
@@ -2729,9 +2729,9 @@
         <v>100</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E95" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F95" s="4" t="s">
@@ -2739,7 +2739,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="7"/>
+      <c r="A96" s="14"/>
       <c r="B96">
         <v>18</v>
       </c>
@@ -2747,9 +2747,9 @@
         <v>101</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="E96" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E96" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F96" s="4" t="s">
@@ -2757,7 +2757,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="7"/>
+      <c r="A97" s="14"/>
       <c r="B97">
         <v>18</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>102</v>
       </c>
       <c r="D97" s="1"/>
-      <c r="E97" s="12">
+      <c r="E97" s="11">
         <v>900</v>
       </c>
       <c r="F97" s="5" t="s">
@@ -2773,7 +2773,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="14" t="s">
         <v>119</v>
       </c>
       <c r="B98">
@@ -2783,7 +2783,7 @@
         <v>26</v>
       </c>
       <c r="D98" s="1"/>
-      <c r="E98" s="10" t="s">
+      <c r="E98" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F98" s="3" t="s">
@@ -2791,7 +2791,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="7"/>
+      <c r="A99" s="14"/>
       <c r="B99">
         <v>19</v>
       </c>
@@ -2799,9 +2799,9 @@
         <v>103</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E99" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="E99" s="10" t="s">
         <v>6</v>
       </c>
       <c r="F99" s="4" t="s">
@@ -2809,7 +2809,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="7"/>
+      <c r="A100" s="14"/>
       <c r="B100">
         <v>19</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>104</v>
       </c>
       <c r="D100" s="1"/>
-      <c r="E100" s="12">
+      <c r="E100" s="11">
         <v>900</v>
       </c>
       <c r="F100" s="5" t="s">
@@ -2825,594 +2825,595 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E101" s="13"/>
+      <c r="E101" s="12"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E102" s="13"/>
+      <c r="E102" s="12"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E103" s="13"/>
+      <c r="E103" s="12"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E104" s="13"/>
+      <c r="E104" s="12"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E105" s="13"/>
+      <c r="E105" s="12"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E106" s="13"/>
+      <c r="E106" s="12"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E107" s="13"/>
+      <c r="E107" s="12"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E108" s="13"/>
+      <c r="E108" s="12"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E109" s="13"/>
+      <c r="E109" s="12"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E110" s="13"/>
+      <c r="E110" s="12"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E111" s="13"/>
+      <c r="E111" s="12"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E112" s="13"/>
+      <c r="E112" s="12"/>
     </row>
     <row r="113" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E113" s="13"/>
+      <c r="E113" s="12"/>
     </row>
     <row r="114" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E114" s="13"/>
+      <c r="E114" s="12"/>
     </row>
     <row r="115" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E115" s="13"/>
+      <c r="E115" s="12"/>
     </row>
     <row r="116" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E116" s="13"/>
+      <c r="E116" s="12"/>
     </row>
     <row r="117" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E117" s="13"/>
+      <c r="E117" s="12"/>
     </row>
     <row r="118" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E118" s="13"/>
+      <c r="E118" s="12"/>
     </row>
     <row r="119" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E119" s="13"/>
+      <c r="E119" s="12"/>
     </row>
     <row r="120" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E120" s="13"/>
+      <c r="E120" s="12"/>
     </row>
     <row r="121" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E121" s="13"/>
+      <c r="E121" s="12"/>
     </row>
     <row r="122" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E122" s="13"/>
+      <c r="E122" s="12"/>
     </row>
     <row r="123" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E123" s="13"/>
+      <c r="E123" s="12"/>
     </row>
     <row r="124" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E124" s="13"/>
+      <c r="E124" s="12"/>
     </row>
     <row r="125" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E125" s="13"/>
+      <c r="E125" s="12"/>
     </row>
     <row r="126" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E126" s="13"/>
+      <c r="E126" s="12"/>
     </row>
     <row r="127" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E127" s="13"/>
+      <c r="E127" s="12"/>
     </row>
     <row r="128" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E128" s="13"/>
+      <c r="E128" s="12"/>
     </row>
     <row r="129" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E129" s="13"/>
+      <c r="E129" s="12"/>
     </row>
     <row r="130" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E130" s="13"/>
+      <c r="E130" s="12"/>
     </row>
     <row r="131" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E131" s="13"/>
+      <c r="E131" s="12"/>
     </row>
     <row r="132" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E132" s="13"/>
+      <c r="E132" s="12"/>
     </row>
     <row r="133" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E133" s="13"/>
+      <c r="E133" s="12"/>
     </row>
     <row r="134" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E134" s="13"/>
+      <c r="E134" s="12"/>
     </row>
     <row r="135" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E135" s="13"/>
+      <c r="E135" s="12"/>
     </row>
     <row r="136" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E136" s="13"/>
+      <c r="E136" s="12"/>
     </row>
     <row r="137" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E137" s="13"/>
+      <c r="E137" s="12"/>
     </row>
     <row r="138" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E138" s="13"/>
+      <c r="E138" s="12"/>
     </row>
     <row r="139" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E139" s="13"/>
+      <c r="E139" s="12"/>
     </row>
     <row r="140" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E140" s="13"/>
+      <c r="E140" s="12"/>
     </row>
     <row r="141" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E141" s="13"/>
+      <c r="E141" s="12"/>
     </row>
     <row r="142" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E142" s="13"/>
+      <c r="E142" s="12"/>
     </row>
     <row r="143" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E143" s="13"/>
+      <c r="E143" s="12"/>
     </row>
     <row r="144" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E144" s="13"/>
+      <c r="E144" s="12"/>
     </row>
     <row r="145" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E145" s="13"/>
+      <c r="E145" s="12"/>
     </row>
     <row r="146" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E146" s="13"/>
+      <c r="E146" s="12"/>
     </row>
     <row r="147" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E147" s="13"/>
+      <c r="E147" s="12"/>
     </row>
     <row r="148" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E148" s="13"/>
+      <c r="E148" s="12"/>
     </row>
     <row r="149" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E149" s="13"/>
+      <c r="E149" s="12"/>
     </row>
     <row r="150" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E150" s="13"/>
+      <c r="E150" s="12"/>
     </row>
     <row r="151" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E151" s="13"/>
+      <c r="E151" s="12"/>
     </row>
     <row r="152" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E152" s="13"/>
+      <c r="E152" s="12"/>
     </row>
     <row r="153" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E153" s="13"/>
+      <c r="E153" s="12"/>
     </row>
     <row r="154" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E154" s="13"/>
+      <c r="E154" s="12"/>
     </row>
     <row r="155" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E155" s="13"/>
+      <c r="E155" s="12"/>
     </row>
     <row r="156" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E156" s="13"/>
+      <c r="E156" s="12"/>
     </row>
     <row r="157" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E157" s="13"/>
+      <c r="E157" s="12"/>
     </row>
     <row r="158" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E158" s="13"/>
+      <c r="E158" s="12"/>
     </row>
     <row r="159" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E159" s="13"/>
+      <c r="E159" s="12"/>
     </row>
     <row r="160" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E160" s="13"/>
+      <c r="E160" s="12"/>
     </row>
     <row r="161" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E161" s="13"/>
+      <c r="E161" s="12"/>
     </row>
     <row r="162" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E162" s="13"/>
+      <c r="E162" s="12"/>
     </row>
     <row r="163" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E163" s="13"/>
+      <c r="E163" s="12"/>
     </row>
     <row r="164" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E164" s="13"/>
+      <c r="E164" s="12"/>
     </row>
     <row r="165" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E165" s="13"/>
+      <c r="E165" s="12"/>
     </row>
     <row r="166" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E166" s="13"/>
+      <c r="E166" s="12"/>
     </row>
     <row r="167" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E167" s="13"/>
+      <c r="E167" s="12"/>
     </row>
     <row r="168" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E168" s="13"/>
+      <c r="E168" s="12"/>
     </row>
     <row r="169" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E169" s="13"/>
+      <c r="E169" s="12"/>
     </row>
     <row r="170" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E170" s="13"/>
+      <c r="E170" s="12"/>
     </row>
     <row r="171" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E171" s="13"/>
+      <c r="E171" s="12"/>
     </row>
     <row r="172" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E172" s="13"/>
+      <c r="E172" s="12"/>
     </row>
     <row r="173" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E173" s="13"/>
+      <c r="E173" s="12"/>
     </row>
     <row r="174" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E174" s="13"/>
+      <c r="E174" s="12"/>
     </row>
     <row r="175" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E175" s="13"/>
+      <c r="E175" s="12"/>
     </row>
     <row r="176" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E176" s="13"/>
+      <c r="E176" s="12"/>
     </row>
     <row r="177" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E177" s="13"/>
+      <c r="E177" s="12"/>
     </row>
     <row r="178" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E178" s="13"/>
+      <c r="E178" s="12"/>
     </row>
     <row r="179" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E179" s="13"/>
+      <c r="E179" s="12"/>
     </row>
     <row r="180" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E180" s="13"/>
+      <c r="E180" s="12"/>
     </row>
     <row r="181" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E181" s="13"/>
+      <c r="E181" s="12"/>
     </row>
     <row r="182" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E182" s="13"/>
+      <c r="E182" s="12"/>
     </row>
     <row r="183" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E183" s="13"/>
+      <c r="E183" s="12"/>
     </row>
     <row r="184" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E184" s="13"/>
+      <c r="E184" s="12"/>
     </row>
     <row r="185" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E185" s="13"/>
+      <c r="E185" s="12"/>
     </row>
     <row r="186" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E186" s="13"/>
+      <c r="E186" s="12"/>
     </row>
     <row r="187" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E187" s="13"/>
+      <c r="E187" s="12"/>
     </row>
     <row r="188" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E188" s="13"/>
+      <c r="E188" s="12"/>
     </row>
     <row r="189" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E189" s="13"/>
+      <c r="E189" s="12"/>
     </row>
     <row r="190" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E190" s="13"/>
+      <c r="E190" s="12"/>
     </row>
     <row r="191" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E191" s="13"/>
+      <c r="E191" s="12"/>
     </row>
     <row r="192" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E192" s="13"/>
+      <c r="E192" s="12"/>
     </row>
     <row r="193" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E193" s="13"/>
+      <c r="E193" s="12"/>
     </row>
     <row r="194" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E194" s="13"/>
+      <c r="E194" s="12"/>
     </row>
     <row r="195" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E195" s="13"/>
+      <c r="E195" s="12"/>
     </row>
     <row r="196" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E196" s="13"/>
+      <c r="E196" s="12"/>
     </row>
     <row r="197" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E197" s="13"/>
+      <c r="E197" s="12"/>
     </row>
     <row r="198" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E198" s="13"/>
+      <c r="E198" s="12"/>
     </row>
     <row r="199" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E199" s="13"/>
+      <c r="E199" s="12"/>
     </row>
     <row r="200" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E200" s="13"/>
+      <c r="E200" s="12"/>
     </row>
     <row r="201" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E201" s="13"/>
+      <c r="E201" s="12"/>
     </row>
     <row r="202" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E202" s="13"/>
+      <c r="E202" s="12"/>
     </row>
     <row r="203" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E203" s="13"/>
+      <c r="E203" s="12"/>
     </row>
     <row r="204" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E204" s="13"/>
+      <c r="E204" s="12"/>
     </row>
     <row r="205" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E205" s="13"/>
+      <c r="E205" s="12"/>
     </row>
     <row r="206" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E206" s="13"/>
+      <c r="E206" s="12"/>
     </row>
     <row r="207" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E207" s="13"/>
+      <c r="E207" s="12"/>
     </row>
     <row r="208" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E208" s="13"/>
+      <c r="E208" s="12"/>
     </row>
     <row r="209" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E209" s="13"/>
+      <c r="E209" s="12"/>
     </row>
     <row r="210" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E210" s="13"/>
+      <c r="E210" s="12"/>
     </row>
     <row r="211" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E211" s="13"/>
+      <c r="E211" s="12"/>
     </row>
     <row r="212" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E212" s="13"/>
+      <c r="E212" s="12"/>
     </row>
     <row r="213" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E213" s="13"/>
+      <c r="E213" s="12"/>
     </row>
     <row r="214" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E214" s="13"/>
+      <c r="E214" s="12"/>
     </row>
     <row r="215" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E215" s="13"/>
+      <c r="E215" s="12"/>
     </row>
     <row r="216" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E216" s="13"/>
+      <c r="E216" s="12"/>
     </row>
     <row r="217" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E217" s="13"/>
+      <c r="E217" s="12"/>
     </row>
     <row r="218" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E218" s="13"/>
+      <c r="E218" s="12"/>
     </row>
     <row r="219" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E219" s="13"/>
+      <c r="E219" s="12"/>
     </row>
     <row r="220" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E220" s="13"/>
+      <c r="E220" s="12"/>
     </row>
     <row r="221" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E221" s="13"/>
+      <c r="E221" s="12"/>
     </row>
     <row r="222" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E222" s="13"/>
+      <c r="E222" s="12"/>
     </row>
     <row r="223" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E223" s="13"/>
+      <c r="E223" s="12"/>
     </row>
     <row r="224" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E224" s="13"/>
+      <c r="E224" s="12"/>
     </row>
     <row r="225" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E225" s="13"/>
+      <c r="E225" s="12"/>
     </row>
     <row r="226" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E226" s="13"/>
+      <c r="E226" s="12"/>
     </row>
     <row r="227" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E227" s="13"/>
+      <c r="E227" s="12"/>
     </row>
     <row r="228" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E228" s="13"/>
+      <c r="E228" s="12"/>
     </row>
     <row r="229" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E229" s="13"/>
+      <c r="E229" s="12"/>
     </row>
     <row r="230" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E230" s="13"/>
+      <c r="E230" s="12"/>
     </row>
     <row r="231" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E231" s="13"/>
+      <c r="E231" s="12"/>
     </row>
     <row r="232" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E232" s="13"/>
+      <c r="E232" s="12"/>
     </row>
     <row r="233" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E233" s="13"/>
+      <c r="E233" s="12"/>
     </row>
     <row r="234" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E234" s="13"/>
+      <c r="E234" s="12"/>
     </row>
     <row r="235" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E235" s="13"/>
+      <c r="E235" s="12"/>
     </row>
     <row r="236" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E236" s="13"/>
+      <c r="E236" s="12"/>
     </row>
     <row r="237" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E237" s="13"/>
+      <c r="E237" s="12"/>
     </row>
     <row r="238" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E238" s="13"/>
+      <c r="E238" s="12"/>
     </row>
     <row r="239" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E239" s="13"/>
+      <c r="E239" s="12"/>
     </row>
     <row r="240" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E240" s="13"/>
+      <c r="E240" s="12"/>
     </row>
     <row r="241" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E241" s="13"/>
+      <c r="E241" s="12"/>
     </row>
     <row r="242" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E242" s="13"/>
+      <c r="E242" s="12"/>
     </row>
     <row r="243" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E243" s="13"/>
+      <c r="E243" s="12"/>
     </row>
     <row r="244" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E244" s="13"/>
+      <c r="E244" s="12"/>
     </row>
     <row r="245" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E245" s="13"/>
+      <c r="E245" s="12"/>
     </row>
     <row r="246" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E246" s="13"/>
+      <c r="E246" s="12"/>
     </row>
     <row r="247" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E247" s="13"/>
+      <c r="E247" s="12"/>
     </row>
     <row r="248" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E248" s="13"/>
+      <c r="E248" s="12"/>
     </row>
     <row r="249" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E249" s="13"/>
+      <c r="E249" s="12"/>
     </row>
     <row r="250" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E250" s="13"/>
+      <c r="E250" s="12"/>
     </row>
     <row r="251" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E251" s="13"/>
+      <c r="E251" s="12"/>
     </row>
     <row r="252" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E252" s="13"/>
+      <c r="E252" s="12"/>
     </row>
     <row r="253" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E253" s="13"/>
+      <c r="E253" s="12"/>
     </row>
     <row r="254" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E254" s="13"/>
+      <c r="E254" s="12"/>
     </row>
     <row r="255" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E255" s="13"/>
+      <c r="E255" s="12"/>
     </row>
     <row r="256" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E256" s="13"/>
+      <c r="E256" s="12"/>
     </row>
     <row r="257" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E257" s="13"/>
+      <c r="E257" s="12"/>
     </row>
     <row r="258" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E258" s="13"/>
+      <c r="E258" s="12"/>
     </row>
     <row r="259" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E259" s="13"/>
+      <c r="E259" s="12"/>
     </row>
     <row r="260" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E260" s="13"/>
+      <c r="E260" s="12"/>
     </row>
     <row r="261" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E261" s="13"/>
+      <c r="E261" s="12"/>
     </row>
     <row r="262" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E262" s="13"/>
+      <c r="E262" s="12"/>
     </row>
     <row r="263" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E263" s="13"/>
+      <c r="E263" s="12"/>
     </row>
     <row r="264" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E264" s="13"/>
+      <c r="E264" s="12"/>
     </row>
     <row r="265" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E265" s="13"/>
+      <c r="E265" s="12"/>
     </row>
     <row r="266" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E266" s="13"/>
+      <c r="E266" s="12"/>
     </row>
     <row r="267" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E267" s="13"/>
+      <c r="E267" s="12"/>
     </row>
     <row r="268" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E268" s="13"/>
+      <c r="E268" s="12"/>
     </row>
     <row r="269" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E269" s="13"/>
+      <c r="E269" s="12"/>
     </row>
     <row r="270" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E270" s="13"/>
+      <c r="E270" s="12"/>
     </row>
     <row r="271" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E271" s="13"/>
+      <c r="E271" s="12"/>
     </row>
     <row r="272" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E272" s="13"/>
+      <c r="E272" s="12"/>
     </row>
     <row r="273" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E273" s="13"/>
+      <c r="E273" s="12"/>
     </row>
     <row r="274" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E274" s="13"/>
+      <c r="E274" s="12"/>
     </row>
     <row r="275" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E275" s="13"/>
+      <c r="E275" s="12"/>
     </row>
     <row r="276" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E276" s="13"/>
+      <c r="E276" s="12"/>
     </row>
     <row r="277" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E277" s="13"/>
+      <c r="E277" s="12"/>
     </row>
     <row r="278" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E278" s="13"/>
+      <c r="E278" s="12"/>
     </row>
     <row r="279" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E279" s="13"/>
+      <c r="E279" s="12"/>
     </row>
     <row r="280" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E280" s="13"/>
+      <c r="E280" s="12"/>
     </row>
     <row r="281" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E281" s="13"/>
+      <c r="E281" s="12"/>
     </row>
     <row r="282" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E282" s="13"/>
+      <c r="E282" s="12"/>
     </row>
     <row r="283" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E283" s="13"/>
+      <c r="E283" s="12"/>
     </row>
     <row r="284" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E284" s="13"/>
+      <c r="E284" s="12"/>
     </row>
     <row r="285" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E285" s="13"/>
+      <c r="E285" s="12"/>
     </row>
     <row r="286" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E286" s="13"/>
+      <c r="E286" s="12"/>
     </row>
     <row r="287" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E287" s="13"/>
+      <c r="E287" s="12"/>
     </row>
     <row r="288" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E288" s="13"/>
+      <c r="E288" s="12"/>
     </row>
     <row r="289" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E289" s="13"/>
+      <c r="E289" s="12"/>
     </row>
     <row r="290" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E290" s="13"/>
+      <c r="E290" s="12"/>
     </row>
     <row r="291" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E291" s="13"/>
+      <c r="E291" s="12"/>
     </row>
     <row r="292" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E292" s="13"/>
+      <c r="E292" s="12"/>
     </row>
     <row r="293" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E293" s="13"/>
+      <c r="E293" s="12"/>
     </row>
     <row r="294" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E294" s="13"/>
+      <c r="E294" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A67:A76"/>
-    <mergeCell ref="A77:A80"/>
-    <mergeCell ref="A81:A87"/>
-    <mergeCell ref="A88:A93"/>
-    <mergeCell ref="A94:A97"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A31:A34"/>
     <mergeCell ref="A98:A100"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A42:A45"/>
@@ -3420,12 +3421,11 @@
     <mergeCell ref="A54:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A67:A76"/>
+    <mergeCell ref="A77:A80"/>
+    <mergeCell ref="A81:A87"/>
+    <mergeCell ref="A88:A93"/>
+    <mergeCell ref="A94:A97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>

<commit_message>
Assigning treatment post vars and fixing dates
</commit_message>
<xml_diff>
--- a/code/lista_homogen_codes_geo.xlsx
+++ b/code/lista_homogen_codes_geo.xlsx
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38:F41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>